<commit_message>
Se actualizan Excels y Script para llenado de datos automático
</commit_message>
<xml_diff>
--- a/Varios/Giros.xlsx
+++ b/Varios/Giros.xlsx
@@ -2130,22 +2130,22 @@
     <t>ORGANIZACIONES Y ÓRGANOS EXTRATERRITORIALES</t>
   </si>
   <si>
-    <t>CODIGO</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>IVA</t>
-  </si>
-  <si>
-    <t>NET</t>
-  </si>
-  <si>
-    <t>TRIBUTA</t>
-  </si>
-  <si>
     <t>Giros</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Iva</t>
+  </si>
+  <si>
+    <t>CatTributaria</t>
+  </si>
+  <si>
+    <t>Internet</t>
   </si>
 </sst>
 </file>
@@ -2164,6 +2164,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2530,7 +2531,7 @@
   <dimension ref="A1:H701"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2540,31 +2541,31 @@
     <col min="3" max="3" width="3.69921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D1" t="s">
         <v>707</v>
       </c>
       <c r="E1" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="F1" t="str">
         <f>CONCATENATE("INSERT INTO ",$H$1," (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO Giros (CODIGO, NOMBRE, IVA, TRIBUTA, NET) VALUES </v>
+        <v xml:space="preserve">INSERT INTO Giros (Codigo, Nombre, Iva, CatTributaria, Internet) VALUES </v>
       </c>
       <c r="H1" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3176,7 +3177,7 @@
         <v>(11240, 'PRODUCCIÓN EN VIVEROS; EXCEPTO ESPECIES FORESTALES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>11250</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>(11313, 'CULTIVO DE UVA DE MESA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>11321</v>
       </c>
@@ -3281,7 +3282,7 @@
         <v>(11321, 'CULTIVO DE FRUTALES EN ÁRBOLES O ARBUSTOS CON CICLO DE VIDA MAYOR A UNA TEMPORADA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>11322</v>
       </c>
@@ -3302,7 +3303,7 @@
         <v>(11322, 'CULTIVO DE FRUTALES MENORES EN PLANTAS CON CICLO DE VIDA DE UNA TEMPORADA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>11330</v>
       </c>
@@ -3365,7 +3366,7 @@
         <v>(12111, 'CRÍA DE GANADO BOVINO PARA LA PRODUCCIÓN LECHERA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>12112</v>
       </c>
@@ -3554,7 +3555,7 @@
         <v>(12240, 'APICULTURA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>12250</v>
       </c>
@@ -3575,7 +3576,7 @@
         <v>(12250, 'RANICULTURA, HELICICULTURA U OTRA ACTIVIDAD CON ANIMALES MENORES O INSECTOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>12290</v>
       </c>
@@ -3638,7 +3639,7 @@
         <v>(14011, 'SERVICIO DE CORTE Y ENFARDADO DE FORRAJE', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>14012</v>
       </c>
@@ -3701,7 +3702,7 @@
         <v>(14014, 'DESTRUCCIÓN DE PLAGAS; PULVERIZACIONES, FUMIGACIONES U OTRAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>14015</v>
       </c>
@@ -3743,7 +3744,7 @@
         <v>(14019, 'OTROS SERVICIOS AGRÍCOLAS N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>14021</v>
       </c>
@@ -3806,7 +3807,7 @@
         <v>(15010, 'CAZA DE MAMÍFEROS MARINOS; EXCEPTO BALLENAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>15090</v>
       </c>
@@ -4058,7 +4059,7 @@
         <v>(51040, 'REPRODUCCIÓN Y CRÍA DE MOLUSCOS Y CRUSTACEOS.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>51090</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>(52020, 'ACTIVIDAD PESQUERA DE BARCOS FACTORÍAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>52030</v>
       </c>
@@ -4142,7 +4143,7 @@
         <v>(52030, 'PESCA ARTESANAL. EXTRACCIÓN DE RECURSOS ACUÁTICOS EN GENERAL; INCLUYE BALLENAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>52040</v>
       </c>
@@ -4163,7 +4164,7 @@
         <v>(52040, 'RECOLECCIÓN DE PRODUCTOS MARINOS, COMO PERLAS NATURALES, ESPONJAS, CORALES Y ALGAS.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>52050</v>
       </c>
@@ -4226,7 +4227,7 @@
         <v>(111000, 'EXTRACCIÓN DE PETRÓLEO CRUDO Y GAS NATURAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>112000</v>
       </c>
@@ -4499,7 +4500,7 @@
         <v>(142900, 'EXPLOTACIÓN DE OTRAS MINAS Y CANTERAS N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>151110</v>
       </c>
@@ -4541,7 +4542,7 @@
         <v>(151120, 'CONSERVACIÓN DE CARNES ROJAS (FRIGORÍFICOS)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>151130</v>
       </c>
@@ -4646,7 +4647,7 @@
         <v>(151222, 'ELABORACIÓN DE CONGELADOS DE PESCADOS Y MARISCOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>151223</v>
       </c>
@@ -4688,7 +4689,7 @@
         <v>(151230, 'ELABORACIÓN DE PRODUCTOS EN BASE A VEGETALES ACUÁTICOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>151300</v>
       </c>
@@ -4730,7 +4731,7 @@
         <v>(151410, 'ELABORACIÓN DE ACEITES Y GRASAS DE ORIGEN VEGETAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>151420</v>
       </c>
@@ -4772,7 +4773,7 @@
         <v>(151430, 'ELABORACIÓN DE ACEITES Y GRASAS DE ORIGEN MARINO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>152010</v>
       </c>
@@ -4814,7 +4815,7 @@
         <v>(152020, 'ELABORACIÓN DE QUESOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>152030</v>
       </c>
@@ -4877,7 +4878,7 @@
         <v>(153120, 'ACTIVIDADES DE MOLIENDA DE ARROZ', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>153190</v>
       </c>
@@ -4919,7 +4920,7 @@
         <v>(153210, 'ELABORACIÓN DE ALMIDONES Y PRODUCTOS DERIVADOS DEL ALMIDÓN', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>153220</v>
       </c>
@@ -5066,7 +5067,7 @@
         <v>(154320, 'FABRICACIÓN DE PRODUCTOS DE CONFITERÍA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>154400</v>
       </c>
@@ -5129,7 +5130,7 @@
         <v>(154920, 'ELABORACIÓN DE LEVADURAS NATURALES O ARTIFICIALES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>154930</v>
       </c>
@@ -5150,7 +5151,7 @@
         <v>(154930, 'ELABORACIÓN DE VINAGRES, MOSTAZAS, MAYONESAS Y CONDIMENTOS EN GENERAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>154990</v>
       </c>
@@ -5192,7 +5193,7 @@
         <v>(155110, 'ELABORACIÓN DE PISCOS (INDUSTRIAS PISQUERAS)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>155120</v>
       </c>
@@ -5276,7 +5277,7 @@
         <v>(155410, 'ELABORACIÓN DE BEBIDAS NO ALCOHÓLICAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>155420</v>
       </c>
@@ -5360,7 +5361,7 @@
         <v>(160090, 'FABRICACIÓN DE OTROS PRODUCTOS DEL TABACO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>171100</v>
       </c>
@@ -5402,7 +5403,7 @@
         <v>(171200, 'ACABADO DE PRODUCTOS TEXTIL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>172100</v>
       </c>
@@ -5465,7 +5466,7 @@
         <v>(172300, 'FABRICACIÓN DE CUERDAS, CORDELES, BRAMANTES Y REDES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>172910</v>
       </c>
@@ -5549,7 +5550,7 @@
         <v>(181010, 'FABRICACIÓN DE PRENDAS DE VESTIR TEXTILES Y SIMILARES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>181020</v>
       </c>
@@ -5654,7 +5655,7 @@
         <v>(191100, 'CURTIDO Y ADOBO DE CUEROS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>191200</v>
       </c>
@@ -5717,7 +5718,7 @@
         <v>(201000, 'ASERRADO Y ACEPILLADURA DE MADERAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>202100</v>
       </c>
@@ -5738,7 +5739,7 @@
         <v>(202100, 'FABRICACIÓN DE TABLEROS, PANELES Y HOJAS DE MADERA PARA ENCHAPADO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>202200</v>
       </c>
@@ -5780,7 +5781,7 @@
         <v>(202300, 'FABRICACIÓN DE RECIPIENTES DE MADERA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>202900</v>
       </c>
@@ -5864,7 +5865,7 @@
         <v>(210129, 'FABRICACIÓN DE PAPEL Y CARTÓN N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>210200</v>
       </c>
@@ -6179,7 +6180,7 @@
         <v>(241110, 'FABRICACIÓN DE CARBÓN VEGETAL, Y BRIQUETAS DE CARBÓN VEGETAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>241190</v>
       </c>
@@ -6221,7 +6222,7 @@
         <v>(241200, 'FABRICACIÓN DE ABONOS Y COMPUESTOS DE NITRÓGENO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>241300</v>
       </c>
@@ -6242,7 +6243,7 @@
         <v>(241300, 'FABRICACIÓN DE PLÁSTICOS EN FORMAS PRIMARIAS Y DE CAUCHO SINTÉTICO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>242100</v>
       </c>
@@ -6263,7 +6264,7 @@
         <v>(242100, 'FABRICACIÓN DE PLAGUICIDAS Y OTROS PRODUCTOS QUÍMICOS DE USO AGROPECUARIO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>242200</v>
       </c>
@@ -6284,7 +6285,7 @@
         <v>(242200, 'FABRICACIÓN DE PINTURAS, BARNICES Y PRODUCTOS DE REVESTIMIENTO SIMILARES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>242300</v>
       </c>
@@ -6305,7 +6306,7 @@
         <v>(242300, 'FABRICACIÓN DE PRODUCTOS FARMACEUTICOS, SUSTANCIAS QUÍMICAS MEDICINALES Y PRODUCTOS BOTÁNICOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>242400</v>
       </c>
@@ -6599,7 +6600,7 @@
         <v>(261090, 'FABRICACIÓN DE ARTÍCULOS DE VIDRIO N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>269101</v>
       </c>
@@ -6620,7 +6621,7 @@
         <v>(269101, 'FABRICACIÓN DE PRODUCTOS DE CERÁMICA NO REFRACTARIA PARA USO NO ESTRUCTURAL CON FINES ORNAMENTALES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>269109</v>
       </c>
@@ -6662,7 +6663,7 @@
         <v>(269200, 'FABRICACIÓN DE PRODUCTOS DE CERÁMICAS REFRACTARIA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>269300</v>
       </c>
@@ -6704,7 +6705,7 @@
         <v>(269400, 'FABRICACIÓN DE CEMENTO, CAL Y YESO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>269510</v>
       </c>
@@ -6809,7 +6810,7 @@
         <v>(269600, 'CORTE, TALLADO Y ACABADO DE LA PIEDRA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>269910</v>
       </c>
@@ -6914,7 +6915,7 @@
         <v>(272020, 'ELABORACIÓN DE PRODUCTOS DE ALUMINIO EN FORMAS PRIMARIAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>272090</v>
       </c>
@@ -7019,7 +7020,7 @@
         <v>(281211, 'FABRICACIÓN DE RECIPIENTES DE GAS COMPRIMIDO O LICUADO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>281219</v>
       </c>
@@ -7061,7 +7062,7 @@
         <v>(281280, 'REPARACIÓN DE TANQUES, DEPÓSITOS Y RECIPIENTES DE METAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>281310</v>
       </c>
@@ -7082,7 +7083,7 @@
         <v>(281310, 'FABRICACIÓN DE GENERADORES DE VAPOR, EXCEPTO CALDERAS DE AGUA CALIENTE PARA CALEFACCIÓN', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>281380</v>
       </c>
@@ -7103,7 +7104,7 @@
         <v>(281380, 'REPARACIÓN DE GENERADORES DE VAPOR, EXCEPTO CALDERAS DE AGUA CALIENTE PARA CALEFACCIÓN CENTRAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>289100</v>
       </c>
@@ -7124,7 +7125,7 @@
         <v>(289100, 'FORJA, PRENSADO, ESTAMPADO Y LAMINADO DE METAL; INCLUYE PULVIMETALURGIA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>289200</v>
       </c>
@@ -7166,7 +7167,7 @@
         <v>(289310, 'FABRICACIÓN DE ARTÍCULOS DE CUCHILLERÍA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>289320</v>
       </c>
@@ -7229,7 +7230,7 @@
         <v>(289990, 'FABRICACIÓN DE OTROS PRODUCTOS ELABORADOS DE METAL N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>291110</v>
       </c>
@@ -7250,7 +7251,7 @@
         <v>(291110, 'FABRICACIÓN DE MOTORES Y TURBINAS, EXCEPTO PARA AERONAVES, VEHÍCULOS AUTOMOTORES Y MOTOCICLETAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>291180</v>
       </c>
@@ -7271,7 +7272,7 @@
         <v>(291180, 'REPARACIÓN DE MOTORES Y TURBINAS, EXCEPTO PARA AERONAVES, VEHÍCULOS AUTOMOTORES Y MOTOCICLETAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>291210</v>
       </c>
@@ -7292,7 +7293,7 @@
         <v>(291210, 'FABRICACIÓN DE BOMBAS, GRIFOS, VÁLVULAS, COMPRESORES, SISTEMAS HIDRÁULICOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>291280</v>
       </c>
@@ -7313,7 +7314,7 @@
         <v>(291280, 'REPARACIÓN DE BOMBAS, COMPRESORES, SISTEMAS HIDRÁULICOS, VÁLVULAS Y ARTÍCULOS DE GRIFERÍA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>291310</v>
       </c>
@@ -7334,7 +7335,7 @@
         <v>(291310, 'FABRICACIÓN DE COJINETES, ENGRANAJES, TRENES DE ENGRANAJES Y PIEZAS DE TRANSMISIÓN', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>291380</v>
       </c>
@@ -7460,7 +7461,7 @@
         <v>(291910, 'FABRICACIÓN DE OTRO TIPO DE MAQUINARIAS DE USO GENERAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>291980</v>
       </c>
@@ -7607,7 +7608,7 @@
         <v>(292380, 'REPARACIÓN DE MAQUINARIA PARA LA INDUSTRIA METALÚRGICA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>292411</v>
       </c>
@@ -7649,7 +7650,7 @@
         <v>(292412, 'FABRICACIÓN DE PARTES PARA MÁQUINAS DE SONDEO O PERFORACIÓN', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>292480</v>
       </c>
@@ -7670,7 +7671,7 @@
         <v>(292480, 'REPARACIÓN DE MAQUINARIA PARA LA EXPLOTACIÓN DE PETRÓLEO, MINAS, CANTERAS, Y OBRAS DE CONSTRUCCIÓN', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>292510</v>
       </c>
@@ -7691,7 +7692,7 @@
         <v>(292510, 'FABRICACIÓN DE MAQUINARIA PARA LA ELABORACIÓN DE ALIMENTOS, BEBIDAS Y TABACOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>292580</v>
       </c>
@@ -7712,7 +7713,7 @@
         <v>(292580, 'REPARACIÓN DE MAQUINARIA PARA LA ELABORACIÓN DE ALIMENTOS, BEBIDAS Y TABACOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>292610</v>
       </c>
@@ -7733,7 +7734,7 @@
         <v>(292610, 'FABRICACIÓN DE MAQUINARIA PARA LA ELABORACIÓN DE PRENDAS TEXTILES, PRENDAS DE VESTIR Y CUEROS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>292680</v>
       </c>
@@ -7859,7 +7860,7 @@
         <v>(293000, 'FABRICACIÓN DE APARATOS DE USO DOMÉSTICO N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>300010</v>
       </c>
@@ -7901,7 +7902,7 @@
         <v>(300020, 'FABRICACIÓN DE MAQUINARIA DE OFICINA, CONTABILIDAD, N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>311010</v>
       </c>
@@ -7922,7 +7923,7 @@
         <v>(311010, 'FABRICACIÓN DE MOTORES, GENERADORES Y TRANSFORMADORES ELÉCTRICOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>311080</v>
       </c>
@@ -8153,7 +8154,7 @@
         <v>(321080, 'REPARACIÓN DE COMPONENTES ELECTRÓNICOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>322010</v>
       </c>
@@ -8174,7 +8175,7 @@
         <v>(322010, 'FABRICACIÓN DE TRANSMISORES DE RADIO Y TELEVISIÓN, APARATOS PARA TELEFONÍA Y TELEGRAFÍA CON HILOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>322080</v>
       </c>
@@ -8195,7 +8196,7 @@
         <v>(322080, 'REPARACIÓN DE TRANSMISORES DE RADIO Y TELEVISIÓN, APARATOS PARA TELEFONÍA Y TELEGRAFÍA CON HILOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>323000</v>
       </c>
@@ -8216,7 +8217,7 @@
         <v>(323000, 'FABRICACIÓN DE RECEPTORES (RADIO Y TV); APARATOS DE GRABACIÓN Y REPRODUCCIÓN (AUDIO Y VIDEO)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>331110</v>
       </c>
@@ -8258,7 +8259,7 @@
         <v>(331120, 'LABORATORIOS DENTALES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>331180</v>
       </c>
@@ -8279,7 +8280,7 @@
         <v>(331180, 'REPARACIÓN DE EQUIPO MÉDICO Y QUIRÚRGICO, Y DE APARATOS ORTOPÉDICOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>331210</v>
       </c>
@@ -8300,7 +8301,7 @@
         <v>(331210, 'FABRICACIÓN DE INSTRUMENTOS Y APARATOS PARA MEDIR, VERIFICAR, ENSAYAR, NAVEGAR Y OTROS FINES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>331280</v>
       </c>
@@ -8363,7 +8364,7 @@
         <v>(331380, 'REPARACIÓN DE EQUIPOS DE CONTROL DE PROCESOS INDUSTRIALES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>332010</v>
       </c>
@@ -8384,7 +8385,7 @@
         <v>(332010, 'FABRICACIÓN Y/O REPARACIÓN DE LENTES Y ARTÍCULOS OFTALMOLÓGICOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>332020</v>
       </c>
@@ -8405,7 +8406,7 @@
         <v>(332020, 'FABRICACIÓN DE INSTRUMENTOS DE OPTICA N.C.P. Y EQUIPOS FOTOGRÁFICOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>332080</v>
       </c>
@@ -8468,7 +8469,7 @@
         <v>(341000, 'FABRICACIÓN DE VEHÍCULOS AUTOMOTORES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>342000</v>
       </c>
@@ -8489,7 +8490,7 @@
         <v>(342000, 'FABRICACIÓN DE CARROCERÍAS PARA VEHÍCULOS AUTOMOTORES; FABRICACIÓN DE REMOLQUES Y SEMI REMOLQUES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>343000</v>
       </c>
@@ -8615,7 +8616,7 @@
         <v>(351280, 'REPARACIÓN DE EMBARCACIONES DE RECREO Y DEPORTES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>352000</v>
       </c>
@@ -8699,7 +8700,7 @@
         <v>(359100, 'FABRICACIÓN DE MOTOCICLETAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>359200</v>
       </c>
@@ -8867,7 +8868,7 @@
         <v>(369400, 'FABRICACIÓN DE JUEGOS Y JUGUETES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>369910</v>
       </c>
@@ -9056,7 +9057,7 @@
         <v>(401011, 'GENERACIÓN HIDROELÉCTRICA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A311" s="1">
         <v>401012</v>
       </c>
@@ -9161,7 +9162,7 @@
         <v>(401030, 'DISTRIBUCIÓN DE ENERGIA ELÉCTRICA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A316" s="1">
         <v>402000</v>
       </c>
@@ -9224,7 +9225,7 @@
         <v>(410000, 'CAPTACIÓN, DEPURACIÓN Y DISTRIBUCIÓN DE AGUA', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A319" s="1">
         <v>451010</v>
       </c>
@@ -9245,7 +9246,7 @@
         <v>(451010, 'PREPARACIÓN DEL TERRENO, EXCAVACIONES Y MOVIMIENTOS DE TIERRAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A320" s="1">
         <v>451020</v>
       </c>
@@ -9329,7 +9330,7 @@
         <v>(453000, 'ACONDICIONAMIENTO DE EDIFICIOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A324" s="1">
         <v>454000</v>
       </c>
@@ -9350,7 +9351,7 @@
         <v>(454000, 'OBRAS MENORES EN CONSTRUCCIÓN (CONTRATISTAS, ALBANILES, CARPINTEROS)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A325" s="1">
         <v>455000</v>
       </c>
@@ -9371,7 +9372,7 @@
         <v>(455000, 'ALQUILER DE EQUIPO DE CONSTRUCCIÓN O DEMOLICIÓN DOTADO DE OPERARIOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A326" s="1">
         <v>501010</v>
       </c>
@@ -9392,7 +9393,7 @@
         <v>(501010, 'VENTA AL POR MAYOR DE VEHÍCULOS AUTOMOTORES (IMPORTACIÓN, DISTRIBUCIÓN) EXCEPTO MOTOCICLETAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A327" s="1">
         <v>501020</v>
       </c>
@@ -9476,7 +9477,7 @@
         <v>(502080, 'MANTENIMIENTO Y REPARACIÓN DE VEHÍCULOS AUTOMOTORES', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A331" s="1">
         <v>503000</v>
       </c>
@@ -9623,7 +9624,7 @@
         <v>(511020, 'CORRETAJE DE GANADO (FERIAS DE GANADO)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A338" s="1">
         <v>511030</v>
       </c>
@@ -9665,7 +9666,7 @@
         <v>(512110, 'VENTA AL POR MAYOR DE ANIMALES VIVOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A340" s="1">
         <v>512120</v>
       </c>
@@ -9833,7 +9834,7 @@
         <v>(512260, 'VENTA AL POR MAYOR DE TABACO Y PRODUCTOS DERIVADOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A348" s="1">
         <v>512290</v>
       </c>
@@ -9854,7 +9855,7 @@
         <v>(512290, 'VENTA AL POR MAYOR DE HUEVOS, LECHE, ABARROTES, Y OTROS ALIMENTOS N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A349" s="1">
         <v>513100</v>
       </c>
@@ -9896,7 +9897,7 @@
         <v>(513910, 'VENTA AL POR MAYOR DE MUEBLES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A351" s="1">
         <v>513920</v>
       </c>
@@ -9917,7 +9918,7 @@
         <v>(513920, 'VENTA AL POR MAYOR DE ARTÍCULOS ELÉCTRICOS Y ELECTRÓNICOS PARA EL HOGAR', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A352" s="1">
         <v>513930</v>
       </c>
@@ -10169,7 +10170,7 @@
         <v>(514200, 'VENTA AL POR MAYOR DE METALES Y MINERALES METALÍFEROS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A364" s="1">
         <v>514310</v>
       </c>
@@ -10190,7 +10191,7 @@
         <v>(514310, 'VENTA AL POR MAYOR DE MADERA NO TRABAJADA Y PRODUCTOS RESULTANTES DE SU ELABORACIÓN PRIMARIA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A365" s="1">
         <v>514320</v>
       </c>
@@ -10274,7 +10275,7 @@
         <v>(514930, 'VENTA AL POR MAYOR DE INSUMOS VETERINARIOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A369" s="1">
         <v>514990</v>
       </c>
@@ -10379,7 +10380,7 @@
         <v>(515004, 'VENTA AL POR MAYOR DE MAQUINARIA PARA LA CONSTRUCCIÓN', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A374" s="1">
         <v>515005</v>
       </c>
@@ -10421,7 +10422,7 @@
         <v>(515006, 'VENTA AL POR MAYOR DE MAQUINARIA PARA TEXTILES Y CUEROS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A376" s="1">
         <v>515007</v>
       </c>
@@ -10442,7 +10443,7 @@
         <v>(515007, 'VENTA AL POR MAYOR DE MÁQUINAS Y EQUIPOS DE OFICINA; INCLUYE MATERIALES CONEXOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A377" s="1">
         <v>515008</v>
       </c>
@@ -10463,7 +10464,7 @@
         <v>(515008, 'VENTA AL POR MAYOR DE MAQUINARIA Y EQUIPO DE TRANSPORTE EXCEPTO VEHÍCULOS AUTOMOTORES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A378" s="1">
         <v>515009</v>
       </c>
@@ -10505,7 +10506,7 @@
         <v>(519000, 'VENTA AL POR MAYOR DE OTROS PRODUCTOS N.C.P.', 1, 1, 0),</v>
       </c>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A380" s="1">
         <v>521111</v>
       </c>
@@ -10526,7 +10527,7 @@
         <v>(521111, 'GRANDES ESTABLECIMIENTOS (VENTA DE ALIMENTOS); HIPERMERCADOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A381" s="1">
         <v>521112</v>
       </c>
@@ -10610,7 +10611,7 @@
         <v>(521300, 'GRANDES TIENDAS - VESTUARIO Y PRODUCTOS PARA EL HOGAR', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A385" s="1">
         <v>521900</v>
       </c>
@@ -10652,7 +10653,7 @@
         <v>(522010, 'VENTA AL POR MENOR DE BEBIDAS Y LICORES (BOTILLERÍAS)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A387" s="1">
         <v>522020</v>
       </c>
@@ -10694,7 +10695,7 @@
         <v>(522030, 'COMERCIO AL POR MENOR DE VERDURAS Y FRUTAS (VERDULERÍA)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A389" s="1">
         <v>522040</v>
       </c>
@@ -10736,7 +10737,7 @@
         <v>(522050, 'VENTA AL POR MENOR DE PRODUCTOS DE PANADERÍA Y PASTELERÍA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A391" s="1">
         <v>522060</v>
       </c>
@@ -10778,7 +10779,7 @@
         <v>(522070, 'VENTA AL POR MENOR DE AVES Y HUEVOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A393" s="1">
         <v>522090</v>
       </c>
@@ -10925,7 +10926,7 @@
         <v>(523210, 'VENTA AL POR MENOR DE CALZADO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A400" s="1">
         <v>523220</v>
       </c>
@@ -10967,7 +10968,7 @@
         <v>(523230, 'VENTA AL POR MENOR DE LANAS, HILOS Y SIMILARES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A402" s="1">
         <v>523240</v>
       </c>
@@ -10988,7 +10989,7 @@
         <v>(523240, 'VENTA AL POR MENOR DE MALETERÍAS, TALABARTERÍAS Y ARTÍCULOS DE CUERO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A403" s="1">
         <v>523250</v>
       </c>
@@ -11009,7 +11010,7 @@
         <v>(523250, 'VENTA AL POR MENOR DE ROPA INTERIOR Y PRENDAS DE USO PERSONAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A404" s="1">
         <v>523290</v>
       </c>
@@ -11030,7 +11031,7 @@
         <v>(523290, 'COMERCIO AL POR MENOR DE TEXTILES PARA EL HOGAR Y OTROS PRODUCTOS TEXTILES N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A405" s="1">
         <v>523310</v>
       </c>
@@ -11051,7 +11052,7 @@
         <v>(523310, 'VENTA AL POR MENOR DE ARTÍCULOS ELECTRODOMÉSTICOS Y ELECTRÓNICOS PARA EL HOGAR', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A406" s="1">
         <v>523320</v>
       </c>
@@ -11093,7 +11094,7 @@
         <v>(523330, 'VENTA AL POR MENOR DE MUEBLES; INCLUYE COLCHONES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A408" s="1">
         <v>523340</v>
       </c>
@@ -11156,7 +11157,7 @@
         <v>(523360, 'VENTA AL POR MENOR DE LÁMPARAS, APLIQUÉS Y SIMILARES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A411" s="1">
         <v>523390</v>
       </c>
@@ -11177,7 +11178,7 @@
         <v>(523390, 'VENTA AL POR MENOR DE APARATOS, ARTÍCULOS, EQUIPO DE USO DOMÉSTICO N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A412" s="1">
         <v>523410</v>
       </c>
@@ -11345,7 +11346,7 @@
         <v>(523923, 'COMERCIO AL POR MENOR DE REVISTAS Y DIARIOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A420" s="1">
         <v>523924</v>
       </c>
@@ -11366,7 +11367,7 @@
         <v>(523924, 'COMERCIO DE ARTÍCULOS DE SUMINISTROS DE OFICINAS Y ARTÍCULOS DE ESCRITORIO EN GENERAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A421" s="1">
         <v>523930</v>
       </c>
@@ -11450,7 +11451,7 @@
         <v>(523943, 'COMERCIO AL POR MENOR DE ARTÍCULOS DEPORTIVOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A425" s="1">
         <v>523950</v>
       </c>
@@ -11492,7 +11493,7 @@
         <v>(523961, 'VENTA AL POR MENOR DE GAS LICUADO EN BOMBONAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A427" s="1">
         <v>523969</v>
       </c>
@@ -11534,7 +11535,7 @@
         <v>(523991, 'COMERCIO AL POR MENOR DE ARTÍCULOS TÍPICOS (ARTESANÍAS)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A429" s="1">
         <v>523992</v>
       </c>
@@ -11576,7 +11577,7 @@
         <v>(523993, 'VENTA AL POR MENOR DE MASCOTAS Y ACCESORIOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A431" s="1">
         <v>523999</v>
       </c>
@@ -11639,7 +11640,7 @@
         <v>(524020, 'COMERCIO AL POR MENOR DE ROPA USADA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A434" s="1">
         <v>524090</v>
       </c>
@@ -11660,7 +11661,7 @@
         <v>(524090, 'COMERCIO AL POR MENOR DE ARTÍCULOS Y ARTEFACTOS USADOS N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A435" s="1">
         <v>525110</v>
       </c>
@@ -11681,7 +11682,7 @@
         <v>(525110, 'VENTA AL POR MENOR EN EMPRESAS DE VENTA A DISTANCIA POR CORREO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A436" s="1">
         <v>525120</v>
       </c>
@@ -11702,7 +11703,7 @@
         <v>(525120, 'VENTA AL POR MENOR EN EMPRESAS DE VENTA A DISTANCIA VÍA TELEFÓNICA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A437" s="1">
         <v>525130</v>
       </c>
@@ -11744,7 +11745,7 @@
         <v>(525200, 'VENTA AL POR MENOR EN PUESTOS DE VENTA Y MERCADOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A439" s="1">
         <v>525911</v>
       </c>
@@ -11765,7 +11766,7 @@
         <v>(525911, 'VENTA AL POR MENOR REALIZADA POR INDEPENDIENTES EN TRANSPORTE PÚBLICO (LEY 20.388)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A440" s="1">
         <v>525919</v>
       </c>
@@ -11828,7 +11829,7 @@
         <v>(525930, 'VENTA AL POR MENOR A CAMBIO DE UNA RETRIBUCIÓN O POR CONTRATA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A443" s="1">
         <v>525990</v>
       </c>
@@ -11912,7 +11913,7 @@
         <v>(526030, 'REPARACIÓN DE RELOJES Y JOYAS', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A447" s="1">
         <v>526090</v>
       </c>
@@ -11996,7 +11997,7 @@
         <v>(551030, 'RESIDENCIALES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A451" s="1">
         <v>551090</v>
       </c>
@@ -12038,7 +12039,7 @@
         <v>(552010, 'RESTAURANTES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A453" s="1">
         <v>552020</v>
       </c>
@@ -12122,7 +12123,7 @@
         <v>(552050, 'SERVICIOS DE BANQUETES, BODAS Y OTRAS CELEBRACIONES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A457" s="1">
         <v>552090</v>
       </c>
@@ -12185,7 +12186,7 @@
         <v>(601002, 'TRANSPORTE DE CARGA POR FERROCARRILES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A460" s="1">
         <v>602110</v>
       </c>
@@ -12206,7 +12207,7 @@
         <v>(602110, 'TRANSPORTE URBANO DE PASAJEROS VÍA FERROCARRIL (INCLUYE METRO)', 0, 1, 1),</v>
       </c>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A461" s="1">
         <v>602120</v>
       </c>
@@ -12311,7 +12312,7 @@
         <v>(602160, 'SERVICIOS DE TRANSPORTE DE TRABAJADORES', 0, 1, 1),</v>
       </c>
     </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A466" s="1">
         <v>602190</v>
       </c>
@@ -12374,7 +12375,7 @@
         <v>(602220, 'SERVICIOS DE TRANSPORTE A TURISTAS', 0, 1, 1),</v>
       </c>
     </row>
-    <row r="469" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A469" s="1">
         <v>602230</v>
       </c>
@@ -12773,7 +12774,7 @@
         <v>(630390, 'OTRAS ACTIVIDADES CONEXAS AL TRANSPORTE N.C.P.', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A488" s="1">
         <v>630400</v>
       </c>
@@ -12857,7 +12858,7 @@
         <v>(641100, 'ACTIVIDADES POSTALES NACIONALES', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="492" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A492" s="1">
         <v>641200</v>
       </c>
@@ -12920,7 +12921,7 @@
         <v>(642020, 'SERVICIOS DE TELEFONÍA MÓVIL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="495" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A495" s="1">
         <v>642030</v>
       </c>
@@ -13319,7 +13320,7 @@
         <v>(659912, 'ADMINISTRADORAS DE FONDOS MUTUOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="514" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A514" s="1">
         <v>659913</v>
       </c>
@@ -13382,7 +13383,7 @@
         <v>(659915, 'ADMINISTRADORAS DE FONDOS PARA OTROS FINES Y/O GENERALES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="517" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A517" s="1">
         <v>659920</v>
       </c>
@@ -13655,7 +13656,7 @@
         <v>(671921, 'ADMINISTRADORA DE TARJETAS DE CRÉDITO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="530" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A530" s="1">
         <v>671929</v>
       </c>
@@ -13718,7 +13719,7 @@
         <v>(671940, 'CASAS DE CAMBIO Y OPERADORES DE DIVISA', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="533" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A533" s="1">
         <v>671990</v>
       </c>
@@ -13781,7 +13782,7 @@
         <v>(672020, 'AGENTES Y LIQUIDADORES DE SEGUROS', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="536" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A536" s="1">
         <v>672090</v>
       </c>
@@ -13823,7 +13824,7 @@
         <v>(701001, 'ARRIENDO DE INMUEBLES AMOBLADOS O CON EQUIPOS Y MAQUINARIAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="538" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A538" s="1">
         <v>701009</v>
       </c>
@@ -13886,7 +13887,7 @@
         <v>(711101, 'ALQUILER DE AUTOS Y CAMIONETAS SIN CHOFER', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="541" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A541" s="1">
         <v>711102</v>
       </c>
@@ -13970,7 +13971,7 @@
         <v>(712100, 'ALQUILER DE MAQUINARIA Y EQUIPO AGROPECUARIO', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="545" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A545" s="1">
         <v>712200</v>
       </c>
@@ -13991,7 +13992,7 @@
         <v>(712200, 'ALQUILER DE MAQUINARIA Y EQUIPO DE CONSTRUCCIÓN E INGENIERÍA CIVIL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="546" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A546" s="1">
         <v>712300</v>
       </c>
@@ -14054,7 +14055,7 @@
         <v>(713010, 'ALQUILER DE BICICLETAS Y ARTÍCULOS PARA DEPORTES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="549" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A549" s="1">
         <v>713020</v>
       </c>
@@ -14075,7 +14076,7 @@
         <v>(713020, 'ARRIENDO DE VIDEOS, JUEGOS DE VIDEO, Y EQUIPOS REPRODUCTORES DE VIDEO, MÚSICA Y SIMILARES', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="550" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A550" s="1">
         <v>713030</v>
       </c>
@@ -14096,7 +14097,7 @@
         <v>(713030, 'ALQUILER DE MOBILIARIO PARA EVENTOS (SILLAS, MESAS, MESONES, VAJILLAS, TOLDOS Y RELACIONADOS)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="551" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A551" s="1">
         <v>713090</v>
       </c>
@@ -14138,7 +14139,7 @@
         <v>(722000, 'ASESORES Y CONSULTORES EN INFORMÁTICA (SOFTWARE)', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="553" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A553" s="1">
         <v>724000</v>
       </c>
@@ -14159,7 +14160,7 @@
         <v>(724000, 'PROCESAMIENTO DE DATOS Y ACTIVIDADES RELACIONADAS CON BASES DE DATOS', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="554" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A554" s="1">
         <v>725000</v>
       </c>
@@ -14201,7 +14202,7 @@
         <v>(726000, 'EMPRESAS DE SERVICIOS INTEGRALES DE INFORMÁTICA', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="556" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A556" s="1">
         <v>731000</v>
       </c>
@@ -14222,7 +14223,7 @@
         <v>(731000, 'INVESTIGACIONES Y DESARROLLO EXPERIMENTAL EN EL CAMPO DE LAS CIENCIAS NATURALES Y LA INGENIERÍA', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="557" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A557" s="1">
         <v>732000</v>
       </c>
@@ -14348,7 +14349,7 @@
         <v>(741190, 'ARBITRAJES, SÍNDICOS, PERITOS Y OTROS', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="563" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A563" s="1">
         <v>741200</v>
       </c>
@@ -14369,7 +14370,7 @@
         <v>(741200, 'ACTIVIDADES DE CONTABILIDAD, TENEDURÍA DE LIBROS Y AUDITORÍA; ASESORAMIENTOS TRIBUTARIOS', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="564" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="564" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A564" s="1">
         <v>741300</v>
       </c>
@@ -14390,7 +14391,7 @@
         <v>(741300, 'INVESTIGACIÓN DE MERCADOS Y REALIZACIÓN DE ENCUESTAS DE OPINIÓN PÚBLICA', NULL, NULL, 1),</v>
       </c>
     </row>
-    <row r="565" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A565" s="1">
         <v>741400</v>
       </c>
@@ -14663,7 +14664,7 @@
         <v>(743002, 'SERVICIOS PERSONALES EN PUBLICIDAD', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="578" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A578" s="1">
         <v>749110</v>
       </c>
@@ -14789,7 +14790,7 @@
         <v>(749229, 'SERVICIOS PERSONALES RELACIONADOS CON SEGURIDAD', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="584" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A584" s="1">
         <v>749310</v>
       </c>
@@ -14957,7 +14958,7 @@
         <v>(749912, 'EVALUACIÓN Y CALIFICACIÓN DEL GRADO DE SOLVENCIA', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="592" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A592" s="1">
         <v>749913</v>
       </c>
@@ -15041,7 +15042,7 @@
         <v>(749929, 'OTROS DISENADORES N.C.P.', NULL, NULL, 1),</v>
       </c>
     </row>
-    <row r="596" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A596" s="1">
         <v>749931</v>
       </c>
@@ -15062,7 +15063,7 @@
         <v>(749931, 'EMPRESAS DE TAQUIGRAFÍA, REPRODUCCIÓN, DESPACHO DE CORRESPONDENCIA, Y OTRAS LABORES DE OFICINA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="597" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="597" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A597" s="1">
         <v>749932</v>
       </c>
@@ -15377,7 +15378,7 @@
         <v>(752200, 'ACTIVIDADES DE DEFENSA', NULL, 1, 0),</v>
       </c>
     </row>
-    <row r="612" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="612" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A612" s="1">
         <v>752300</v>
       </c>
@@ -15398,7 +15399,7 @@
         <v>(752300, 'ACTIVIDADES DE MANTENIMIENTO DEL ORDEN PÚBLICO Y DE SEGURIDAD', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="613" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="613" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A613" s="1">
         <v>753010</v>
       </c>
@@ -15440,7 +15441,7 @@
         <v>(753020, 'CAJAS DE COMPENSACIÓN', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="615" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="615" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A615" s="1">
         <v>753090</v>
       </c>
@@ -15503,7 +15504,7 @@
         <v>(801020, 'ESTABLECIMIENTOS DE ENSEÑANZA PRIMARIA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="618" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="618" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A618" s="1">
         <v>802100</v>
       </c>
@@ -15524,7 +15525,7 @@
         <v>(802100, 'ESTABLECIMIENTOS DE ENSEÑANZA SECUNDARIA DE FORMACIÓN GENERAL', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="619" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="619" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A619" s="1">
         <v>802200</v>
       </c>
@@ -15608,7 +15609,7 @@
         <v>(803030, 'CENTROS DE FORMACIÓN TÉCNICA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="623" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="623" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A623" s="1">
         <v>809010</v>
       </c>
@@ -15650,7 +15651,7 @@
         <v>(809020, 'ESTABLECIMIENTOS DE ENSEÑANZA PREUNIVERSITARIA', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="625" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="625" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A625" s="1">
         <v>809030</v>
       </c>
@@ -15734,7 +15735,7 @@
         <v>(851110, 'HOSPITALES Y CLÍNICAS', 1, 1, 0),</v>
       </c>
     </row>
-    <row r="629" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="629" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A629" s="1">
         <v>851120</v>
       </c>
@@ -15776,7 +15777,7 @@
         <v>(851211, 'SERVICIOS DE MÉDICOS EN FORMA INDEPENDIENTE', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="631" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="631" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A631" s="1">
         <v>851212</v>
       </c>
@@ -15881,7 +15882,7 @@
         <v>(851920, 'OTROS PROFESIONALES DE LA SALUD', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="636" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="636" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A636" s="1">
         <v>851990</v>
       </c>
@@ -15944,7 +15945,7 @@
         <v>(852021, 'SERVICIOS DE MÉDICOS VETERINARIOS EN FORMA INDEPENDIENTE', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="639" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="639" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A639" s="1">
         <v>852029</v>
       </c>
@@ -16133,7 +16134,7 @@
         <v>(900090, 'OTRAS ACTIVIDADES DE MANEJO DE DESPERDICIOS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="648" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="648" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A648" s="1">
         <v>911100</v>
       </c>
@@ -16301,7 +16302,7 @@
         <v>(919920, 'CLUBES SOCIALES', NULL, 1, 0),</v>
       </c>
     </row>
-    <row r="656" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="656" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A656" s="1">
         <v>919930</v>
       </c>
@@ -16448,7 +16449,7 @@
         <v>(921320, 'ACTIVIDADES DE RADIO', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="663" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="663" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A663" s="1">
         <v>921411</v>
       </c>
@@ -16511,7 +16512,7 @@
         <v>(921420, 'ACTIVIDADES EMPRESARIALES DE ARTISTAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="666" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="666" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A666" s="1">
         <v>921430</v>
       </c>
@@ -16532,7 +16533,7 @@
         <v>(921430, 'ACTIVIDADES ARTÍSTICAS; FUNCIONES DE ARTISTAS, ACTORES, MÚSICOS, CONFERENCISTAS, OTROS', 0, 2, 1),</v>
       </c>
     </row>
-    <row r="667" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="667" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A667" s="1">
         <v>921490</v>
       </c>
@@ -16721,7 +16722,7 @@
         <v>(923100, 'ACTIVIDADES DE BIBLIOTECAS Y ARCHIVOS', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="676" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="676" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A676" s="1">
         <v>923200</v>
       </c>
@@ -16742,7 +16743,7 @@
         <v>(923200, 'ACTIVIDADES DE MUSEOS Y PRESERVACIÓN DE LUGARES Y EDIFICIOS HISTÓRICOS', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="677" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="677" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A677" s="1">
         <v>923300</v>
       </c>
@@ -16763,7 +16764,7 @@
         <v>(923300, 'ACTIVIDADES DE JARDINES BOTÁNICOS Y ZOOLÓGICOS Y DE PARQUES NACIONALES', NULL, 1, 1),</v>
       </c>
     </row>
-    <row r="678" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="678" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A678" s="1">
         <v>924110</v>
       </c>
@@ -17036,7 +17037,7 @@
         <v>(924990, 'OTROS SERVICIOS DE DIVERSIÓN Y ESPARCIMIENTOS N.C.P.', NULL, NULL, 1),</v>
       </c>
     </row>
-    <row r="691" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="691" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A691" s="1">
         <v>930100</v>
       </c>
@@ -17141,7 +17142,7 @@
         <v>(930330, 'SERVICIOS DE CARROZAS FÚNEBRES (TRANSPORTE DE CADÁVERES)', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="696" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="696" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A696" s="1">
         <v>930390</v>
       </c>
@@ -17162,7 +17163,7 @@
         <v>(930390, 'OTRAS ACTIVIDADES DE SERVICIOS FUNERARIOS Y OTRAS ACTIVIDADES CONEXAS', 1, 1, 1),</v>
       </c>
     </row>
-    <row r="697" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="697" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A697" s="1">
         <v>930910</v>
       </c>
@@ -17272,6 +17273,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>